<commit_message>
Revert "added requirement openpyxl"
This reverts commit d2c8dd83d73716afb342fbfda9d886f1b3dfd1ca.
</commit_message>
<xml_diff>
--- a/test_file_xlsx.xlsx
+++ b/test_file_xlsx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian.Atlasovich\Documents\Julian\projects\22-05-20_file-validator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian.Atlasovich\Documents\Julian\projects\file-validator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA241CB9-6E0D-4AFC-8636-29886563B2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE7BCF1-4190-4234-8099-74E9858FE059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_file" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
   <si>
     <t>customer_id</t>
   </si>
@@ -35,6 +35,9 @@
     <t>age</t>
   </si>
   <si>
+    <t>sex</t>
+  </si>
+  <si>
     <t>customer_type</t>
   </si>
   <si>
@@ -47,6 +50,9 @@
     <t xml:space="preserve">Hampton </t>
   </si>
   <si>
+    <t>Male</t>
+  </si>
+  <si>
     <t>type1</t>
   </si>
   <si>
@@ -59,6 +65,9 @@
     <t>Miyake</t>
   </si>
   <si>
+    <t>Other</t>
+  </si>
+  <si>
     <t>type3</t>
   </si>
   <si>
@@ -69,6 +78,9 @@
   </si>
   <si>
     <t>Majewska</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
   <si>
     <t>7951ABCD</t>
@@ -1149,15 +1161,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1173,84 +1183,99 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D5">
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D6">
         <v>39</v>
@@ -1258,33 +1283,39 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D8">
         <v>51</v>
@@ -1292,33 +1323,39 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D10">
         <v>82</v>
@@ -1326,67 +1363,79 @@
       <c r="E10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D11">
         <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D12">
         <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D13">
         <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>48</v>
@@ -1394,50 +1443,59 @@
       <c r="E14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D15">
         <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D16">
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D17">
         <v>35</v>
@@ -1445,220 +1503,262 @@
       <c r="E17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D18">
         <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D19">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D20">
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D21">
         <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D22">
         <v>150</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D23">
         <v>37</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D24">
         <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D25">
         <v>63</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D26">
         <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D27">
         <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D28">
         <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D29">
         <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D30">
         <v>61</v>
       </c>
       <c r="E30" t="s">
         <v>19</v>
+      </c>
+      <c r="F30" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1668,23 +1768,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E916B8AC-99A4-4B66-8E26-99263FE2BDB8}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1706,50 +1806,6 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "added requirement openpyxl""
This reverts commit 55de75f14b612d0fdf030743bc311ccc734f5a0f.
</commit_message>
<xml_diff>
--- a/test_file_xlsx.xlsx
+++ b/test_file_xlsx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian.Atlasovich\Documents\Julian\projects\file-validator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian.Atlasovich\Documents\Julian\projects\22-05-20_file-validator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE7BCF1-4190-4234-8099-74E9858FE059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA241CB9-6E0D-4AFC-8636-29886563B2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_file" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
   <si>
     <t>customer_id</t>
   </si>
@@ -35,9 +35,6 @@
     <t>age</t>
   </si>
   <si>
-    <t>sex</t>
-  </si>
-  <si>
     <t>customer_type</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
     <t xml:space="preserve">Hampton </t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
     <t>type1</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
     <t>Miyake</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>type3</t>
   </si>
   <si>
@@ -78,9 +69,6 @@
   </si>
   <si>
     <t>Majewska</t>
-  </si>
-  <si>
-    <t>Female</t>
   </si>
   <si>
     <t>7951ABCD</t>
@@ -1161,13 +1149,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1183,99 +1173,84 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
       <c r="D3">
         <v>40</v>
       </c>
       <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="C4" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
       <c r="D4">
         <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>39</v>
@@ -1283,39 +1258,33 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>51</v>
@@ -1323,39 +1292,33 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D10">
         <v>82</v>
@@ -1363,79 +1326,67 @@
       <c r="E10" t="s">
         <v>19</v>
       </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D11">
         <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D12">
         <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D13">
         <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D14">
         <v>48</v>
@@ -1443,59 +1394,50 @@
       <c r="E14" t="s">
         <v>19</v>
       </c>
-      <c r="F14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15">
         <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D17">
         <v>35</v>
@@ -1503,262 +1445,220 @@
       <c r="E17" t="s">
         <v>19</v>
       </c>
-      <c r="F17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D18">
         <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D19">
         <v>51</v>
       </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D20">
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D21">
         <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D22">
         <v>150</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D23">
         <v>37</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D24">
         <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D25">
         <v>63</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D26">
         <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D27">
         <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D28">
         <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D29">
         <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D30">
         <v>61</v>
       </c>
       <c r="E30" t="s">
         <v>19</v>
-      </c>
-      <c r="F30" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1768,23 +1668,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E916B8AC-99A4-4B66-8E26-99263FE2BDB8}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1806,6 +1706,50 @@
         <v>3</v>
       </c>
       <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Revert "added requirement openpyxl"""
This reverts commit 544b0cbb969dee96e5e91fbd401979405ef5eab5.
</commit_message>
<xml_diff>
--- a/test_file_xlsx.xlsx
+++ b/test_file_xlsx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian.Atlasovich\Documents\Julian\projects\22-05-20_file-validator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian.Atlasovich\Documents\Julian\projects\file-validator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA241CB9-6E0D-4AFC-8636-29886563B2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE7BCF1-4190-4234-8099-74E9858FE059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_file" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
   <si>
     <t>customer_id</t>
   </si>
@@ -35,6 +35,9 @@
     <t>age</t>
   </si>
   <si>
+    <t>sex</t>
+  </si>
+  <si>
     <t>customer_type</t>
   </si>
   <si>
@@ -47,6 +50,9 @@
     <t xml:space="preserve">Hampton </t>
   </si>
   <si>
+    <t>Male</t>
+  </si>
+  <si>
     <t>type1</t>
   </si>
   <si>
@@ -59,6 +65,9 @@
     <t>Miyake</t>
   </si>
   <si>
+    <t>Other</t>
+  </si>
+  <si>
     <t>type3</t>
   </si>
   <si>
@@ -69,6 +78,9 @@
   </si>
   <si>
     <t>Majewska</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
   <si>
     <t>7951ABCD</t>
@@ -1149,15 +1161,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1173,84 +1183,99 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D5">
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D6">
         <v>39</v>
@@ -1258,33 +1283,39 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D8">
         <v>51</v>
@@ -1292,33 +1323,39 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D10">
         <v>82</v>
@@ -1326,67 +1363,79 @@
       <c r="E10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D11">
         <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D12">
         <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D13">
         <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>48</v>
@@ -1394,50 +1443,59 @@
       <c r="E14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D15">
         <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D16">
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D17">
         <v>35</v>
@@ -1445,220 +1503,262 @@
       <c r="E17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D18">
         <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D19">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D20">
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D21">
         <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D22">
         <v>150</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D23">
         <v>37</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D24">
         <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D25">
         <v>63</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D26">
         <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D27">
         <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D28">
         <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D29">
         <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D30">
         <v>61</v>
       </c>
       <c r="E30" t="s">
         <v>19</v>
+      </c>
+      <c r="F30" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1668,23 +1768,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E916B8AC-99A4-4B66-8E26-99263FE2BDB8}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1706,50 +1806,6 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "added requirement openpyxl""""
This reverts commit 7279a7caefcbca587ab3209c901da14274e376a5.
</commit_message>
<xml_diff>
--- a/test_file_xlsx.xlsx
+++ b/test_file_xlsx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian.Atlasovich\Documents\Julian\projects\file-validator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian.Atlasovich\Documents\Julian\projects\22-05-20_file-validator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE7BCF1-4190-4234-8099-74E9858FE059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA241CB9-6E0D-4AFC-8636-29886563B2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_file" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
   <si>
     <t>customer_id</t>
   </si>
@@ -35,9 +35,6 @@
     <t>age</t>
   </si>
   <si>
-    <t>sex</t>
-  </si>
-  <si>
     <t>customer_type</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
     <t xml:space="preserve">Hampton </t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
     <t>type1</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
     <t>Miyake</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>type3</t>
   </si>
   <si>
@@ -78,9 +69,6 @@
   </si>
   <si>
     <t>Majewska</t>
-  </si>
-  <si>
-    <t>Female</t>
   </si>
   <si>
     <t>7951ABCD</t>
@@ -1161,13 +1149,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1183,99 +1173,84 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
       <c r="D3">
         <v>40</v>
       </c>
       <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="C4" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
       <c r="D4">
         <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>39</v>
@@ -1283,39 +1258,33 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>51</v>
@@ -1323,39 +1292,33 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D10">
         <v>82</v>
@@ -1363,79 +1326,67 @@
       <c r="E10" t="s">
         <v>19</v>
       </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D11">
         <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D12">
         <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D13">
         <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D14">
         <v>48</v>
@@ -1443,59 +1394,50 @@
       <c r="E14" t="s">
         <v>19</v>
       </c>
-      <c r="F14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15">
         <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D17">
         <v>35</v>
@@ -1503,262 +1445,220 @@
       <c r="E17" t="s">
         <v>19</v>
       </c>
-      <c r="F17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D18">
         <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D19">
         <v>51</v>
       </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D20">
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D21">
         <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D22">
         <v>150</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D23">
         <v>37</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D24">
         <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D25">
         <v>63</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D26">
         <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D27">
         <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D28">
         <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D29">
         <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D30">
         <v>61</v>
       </c>
       <c r="E30" t="s">
         <v>19</v>
-      </c>
-      <c r="F30" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1768,23 +1668,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E916B8AC-99A4-4B66-8E26-99263FE2BDB8}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1806,6 +1706,50 @@
         <v>3</v>
       </c>
       <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed numeric check first
</commit_message>
<xml_diff>
--- a/test_file_xlsx.xlsx
+++ b/test_file_xlsx.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian.Atlasovich\Documents\Julian\projects\22-05-20_file-validator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA241CB9-6E0D-4AFC-8636-29886563B2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E235E6FB-B59C-46CC-A8B3-7D2A4286B6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test_file" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="customers" sheetId="1" r:id="rId1"/>
+    <sheet name="companies" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="110">
   <si>
     <t>customer_id</t>
   </si>
@@ -302,13 +302,55 @@
     <t>Gonnel</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
+    <t>company_id</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>company_type</t>
+  </si>
+  <si>
+    <t>employee_count</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>company1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">company3 </t>
+  </si>
+  <si>
+    <t>company2</t>
+  </si>
+  <si>
+    <t>company4</t>
+  </si>
+  <si>
+    <t>social media</t>
+  </si>
+  <si>
+    <t>finance</t>
+  </si>
+  <si>
+    <t>sports</t>
+  </si>
+  <si>
+    <t>company5</t>
+  </si>
+  <si>
+    <t>a6</t>
+  </si>
+  <si>
+    <t>a5</t>
   </si>
 </sst>
 </file>
@@ -1151,8 +1193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1668,15 +1710,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E916B8AC-99A4-4B66-8E26-99263FE2BDB8}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -1686,71 +1728,92 @@
       <c r="C1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
+      <c r="D1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7">
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>